<commit_message>
Added areas for internal plastering
</commit_message>
<xml_diff>
--- a/Underfloor Heating/UFH.xlsx
+++ b/Underfloor Heating/UFH.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\ChadHouse\Underfloor Heating\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0BA78106-EC2C-4FDB-A936-841D1FF9A9C2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1365" yWindow="0" windowWidth="28800" windowHeight="11685"/>
+    <workbookView xWindow="1370" yWindow="0" windowWidth="28800" windowHeight="11690" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -71,7 +72,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -362,15 +363,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -385,6 +377,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -664,48 +665,48 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="16" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="11" t="s">
+      <c r="B1" s="18"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="12"/>
-      <c r="F1" s="13"/>
-    </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
+      <c r="E1" s="18"/>
+      <c r="F1" s="19"/>
+    </row>
+    <row r="2" spans="1:6" s="1" customFormat="1" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>5.5750000000000002</v>
       </c>
@@ -726,7 +727,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="6">
         <v>12.3</v>
       </c>
@@ -746,50 +747,50 @@
         <v>6.7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="8">
-        <f>A3*A4</f>
+        <f t="shared" ref="A5:F5" si="0">A3*A4</f>
         <v>68.572500000000005</v>
       </c>
       <c r="B5" s="9">
-        <f>B3*B4</f>
+        <f t="shared" si="0"/>
         <v>48.708000000000006</v>
       </c>
       <c r="C5" s="10">
-        <f>C3*C4</f>
+        <f t="shared" si="0"/>
         <v>46.550000000000004</v>
       </c>
       <c r="D5" s="8">
-        <f>D3*D4</f>
+        <f t="shared" si="0"/>
         <v>48.708000000000006</v>
       </c>
       <c r="E5" s="9">
-        <f>E3*E4</f>
+        <f t="shared" si="0"/>
         <v>77.804999999999993</v>
       </c>
       <c r="F5" s="10">
-        <f>F3*F4</f>
+        <f t="shared" si="0"/>
         <v>10.050000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C6">
         <f>SUM(A5:C5)</f>
         <v>163.83050000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="18" t="s">
+    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="15" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="19">
+    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="16">
         <f>SUM(A5:F5)</f>
         <v>300.39350000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -797,17 +798,17 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>13</v>
       </c>

</xml_diff>